<commit_message>
added bgm and fixed notes timing
</commit_message>
<xml_diff>
--- a/RapZapSnap/Assets/Chew/script/Excel Related/NotesData.xlsx
+++ b/RapZapSnap/Assets/Chew/script/Excel Related/NotesData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="36" windowWidth="23256" windowHeight="12576" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-300" windowWidth="11430" windowHeight="5115" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Phrase1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="15">
   <si>
     <t>delaytime</t>
     <phoneticPr fontId="1"/>
@@ -67,6 +67,10 @@
   <si>
     <t>LeftArrow</t>
   </si>
+  <si>
+    <t>TriangleKey</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -89,7 +93,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,13 +106,34 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -117,11 +142,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -425,13 +456,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
@@ -464,25 +495,25 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>11.3</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1.2</v>
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>-8.4</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>4.4000000000000004</v>
+        <v>-4.5</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
@@ -490,25 +521,25 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-6.5</v>
+        <v>-11</v>
       </c>
       <c r="C3">
-        <v>-6.5</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>-3.6</v>
+        <v>6</v>
       </c>
       <c r="E3">
-        <v>4.4000000000000004</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
@@ -516,25 +547,25 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-12</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>-7</v>
       </c>
       <c r="D4">
-        <v>-1.35</v>
+        <v>-8.6999999999999993</v>
       </c>
       <c r="E4">
-        <v>4.4000000000000004</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
@@ -542,25 +573,25 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>2.6</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>-7.6</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="D5">
-        <v>7.8</v>
+        <v>-3.85</v>
       </c>
       <c r="E5">
-        <v>4.4000000000000004</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
@@ -568,22 +599,22 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-8.4</v>
+        <v>-1.5</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>-7</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>-1.5</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H6" t="s">
         <v>12</v>
@@ -594,25 +625,25 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-7.4</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>7</v>
+        <v>-7</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E7">
-        <v>-1</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
@@ -620,48 +651,36 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1.5</v>
+        <v>-11</v>
       </c>
       <c r="C8">
-        <v>-7</v>
+        <v>3.3</v>
       </c>
       <c r="D8">
-        <v>-8.4</v>
+        <v>6</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>7.8</v>
-      </c>
-      <c r="C9">
-        <v>6.5</v>
-      </c>
-      <c r="D9">
-        <v>-4.2</v>
-      </c>
-      <c r="E9">
-        <v>2.7</v>
-      </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H9" t="s">
         <v>11</v>
@@ -672,25 +691,25 @@
         <v>9</v>
       </c>
       <c r="B10">
+        <v>11</v>
+      </c>
+      <c r="C10">
         <v>3.5</v>
       </c>
-      <c r="C10">
-        <v>-7</v>
-      </c>
       <c r="D10">
-        <v>-8.4</v>
+        <v>-8.65</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
@@ -698,22 +717,22 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>-7.3</v>
+        <v>-4.3</v>
       </c>
       <c r="C11">
-        <v>7</v>
+        <v>-7</v>
       </c>
       <c r="D11">
-        <v>-7.3</v>
+        <v>-4.3</v>
       </c>
       <c r="E11">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H11" t="s">
         <v>12</v>
@@ -724,25 +743,25 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>-11.5</v>
+        <v>11</v>
       </c>
       <c r="C12">
-        <v>4.4000000000000004</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>-7.3</v>
+        <v>-8.6</v>
       </c>
       <c r="E12">
-        <v>-4.5</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
@@ -750,25 +769,25 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>11.3</v>
+        <v>11</v>
       </c>
       <c r="C13">
-        <v>4.4000000000000004</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="D13">
-        <v>4.8</v>
+        <v>-7.5</v>
       </c>
       <c r="E13">
-        <v>-4.5</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
@@ -776,25 +795,25 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>-11.5</v>
+        <v>11</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>-4.5</v>
       </c>
       <c r="D14">
-        <v>3.75</v>
+        <v>-7.5</v>
       </c>
       <c r="E14">
-        <v>3.4</v>
+        <v>-4.5</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
@@ -802,25 +821,25 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>11.3</v>
+        <v>4.7</v>
       </c>
       <c r="C15">
-        <v>4.4000000000000004</v>
+        <v>7</v>
       </c>
       <c r="D15">
-        <v>4.25</v>
+        <v>4.7</v>
       </c>
       <c r="E15">
-        <v>-1</v>
+        <v>-4.5</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
@@ -828,48 +847,36 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>3.75</v>
       </c>
       <c r="C16">
-        <v>-6.5</v>
+        <v>-7</v>
       </c>
       <c r="D16">
-        <v>-5.3</v>
+        <v>3.75</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
-        <v>-11.3</v>
-      </c>
-      <c r="C17">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D17">
-        <v>-5.3</v>
-      </c>
-      <c r="E17">
-        <v>-3.3</v>
-      </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H17" t="s">
         <v>12</v>
@@ -880,31 +887,57 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C18">
-        <v>7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D18">
-        <v>-4.4000000000000004</v>
+        <v>-5.5</v>
       </c>
       <c r="E18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>11</v>
+      </c>
+      <c r="C19">
         <v>-1</v>
       </c>
-      <c r="F18">
-        <v>2</v>
-      </c>
-      <c r="G18">
-        <v>1.5</v>
-      </c>
-      <c r="H18" t="s">
-        <v>9</v>
+      <c r="D19">
+        <v>-4.5</v>
+      </c>
+      <c r="E19">
+        <v>-1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H19">
       <formula1>"CircleKey,CrossKey,TriangleKey,UpArrow,DownArrow,LeftArrow"</formula1>
     </dataValidation>
   </dataValidations>
@@ -915,13 +948,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -953,52 +986,52 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>7</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
         <v>-7</v>
       </c>
-      <c r="D2">
-        <v>-8.3000000000000007</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
         <v>4.4000000000000004</v>
       </c>
-      <c r="F2">
-        <v>0.5</v>
-      </c>
-      <c r="G2">
-        <v>1.5</v>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>11</v>
-      </c>
-      <c r="C3">
-        <v>-0.7</v>
-      </c>
-      <c r="D3">
-        <v>-8.3000000000000007</v>
-      </c>
-      <c r="E3">
-        <v>-0.7</v>
-      </c>
-      <c r="F3">
-        <v>2.5</v>
-      </c>
-      <c r="G3">
+      <c r="B3" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3">
+        <v>-6.8</v>
+      </c>
+      <c r="E3" s="3">
+        <v>-2.7</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1006,25 +1039,25 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>-2.7</v>
+        <v>-7</v>
       </c>
       <c r="D4">
-        <v>-6.8</v>
+        <v>-8.3000000000000007</v>
       </c>
       <c r="E4">
-        <v>-2.7</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
         <v>2</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1032,16 +1065,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1.2</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>-0.7</v>
       </c>
       <c r="D5">
-        <v>1.2</v>
+        <v>-8.3000000000000007</v>
       </c>
       <c r="E5">
-        <v>-4.2</v>
+        <v>-0.7</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1050,7 +1083,7 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1058,16 +1091,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-7</v>
+        <v>11</v>
       </c>
       <c r="C6">
-        <v>-7</v>
+        <v>-2.7</v>
       </c>
       <c r="D6">
-        <v>-7</v>
+        <v>-6.8</v>
       </c>
       <c r="E6">
-        <v>4.5</v>
+        <v>-2.7</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1076,13 +1109,25 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7">
+        <v>1.2</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>1.2</v>
+      </c>
+      <c r="E7">
+        <v>-4.2</v>
+      </c>
       <c r="F7">
         <v>1</v>
       </c>
@@ -1090,7 +1135,7 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1098,16 +1143,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>-4.4000000000000004</v>
+        <v>-7</v>
       </c>
       <c r="C8">
         <v>-7</v>
       </c>
       <c r="D8">
-        <v>-4.4000000000000004</v>
+        <v>-7</v>
       </c>
       <c r="E8">
-        <v>2.75</v>
+        <v>4.5</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1116,27 +1161,15 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>0.9</v>
-      </c>
-      <c r="D9">
-        <v>-4.4000000000000004</v>
-      </c>
-      <c r="E9">
-        <v>0.9</v>
-      </c>
       <c r="F9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -1149,11 +1182,17 @@
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>-4.4000000000000004</v>
+      </c>
+      <c r="C10">
+        <v>-7</v>
+      </c>
       <c r="D10">
-        <v>-7</v>
+        <v>-4.4000000000000004</v>
       </c>
       <c r="E10">
-        <v>-0.3</v>
+        <v>2.75</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1162,7 +1201,7 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1173,39 +1212,33 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>-0.9</v>
+        <v>0.9</v>
       </c>
       <c r="D11">
-        <v>-2</v>
+        <v>-4.4000000000000004</v>
       </c>
       <c r="E11">
-        <v>-0.9</v>
+        <v>0.9</v>
       </c>
       <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
         <v>2</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>-11</v>
-      </c>
-      <c r="C12">
-        <v>-4.4000000000000004</v>
-      </c>
       <c r="D12">
-        <v>8.6</v>
+        <v>-7</v>
       </c>
       <c r="E12">
-        <v>4.5</v>
+        <v>-0.3</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1214,7 +1247,7 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1222,25 +1255,25 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>-11</v>
+        <v>11</v>
       </c>
       <c r="C13">
-        <v>4.4000000000000004</v>
+        <v>-0.9</v>
       </c>
       <c r="D13">
-        <v>8.6</v>
+        <v>-2</v>
       </c>
       <c r="E13">
-        <v>-4.5</v>
+        <v>-0.9</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1251,13 +1284,13 @@
         <v>-11</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>-4.4000000000000004</v>
       </c>
       <c r="D14">
-        <v>7.5</v>
+        <v>8.6</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1266,21 +1299,33 @@
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15">
+        <v>-11</v>
+      </c>
+      <c r="C15">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D15">
+        <v>8.6</v>
+      </c>
+      <c r="E15">
+        <v>-4.5</v>
+      </c>
       <c r="F15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1288,16 +1333,16 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>-2.2000000000000002</v>
+        <v>-11</v>
       </c>
       <c r="C16">
-        <v>-7</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>-2.2000000000000002</v>
+        <v>7.5</v>
       </c>
       <c r="E16">
-        <v>4.4000000000000004</v>
+        <v>2</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1306,39 +1351,79 @@
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="C18">
+        <v>-7</v>
+      </c>
+      <c r="D18">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="E18">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
         <v>-11</v>
       </c>
-      <c r="C17">
+      <c r="C19">
         <v>1.2</v>
       </c>
-      <c r="D17">
+      <c r="D19">
         <v>-0.8</v>
       </c>
-      <c r="E17">
+      <c r="E19">
         <v>1.2</v>
       </c>
-      <c r="F17">
-        <v>2</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H19">
       <formula1>"CircleKey,CrossKey,TriangleKey,UpArrow,DownArrow,LeftArrow"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1348,13 +1433,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="6" max="6" width="7.5" customWidth="1"/>
   </cols>
@@ -1389,52 +1474,52 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>7.8</v>
-      </c>
-      <c r="C2">
-        <v>-7</v>
-      </c>
-      <c r="D2">
-        <v>-8.3000000000000007</v>
-      </c>
-      <c r="E2">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="F2">
-        <v>0.5</v>
-      </c>
-      <c r="G2">
-        <v>1.5</v>
+      <c r="B2" s="2">
+        <v>-3.8</v>
+      </c>
+      <c r="C2" s="2">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2">
+        <v>7.6</v>
+      </c>
+      <c r="E2" s="2">
+        <v>-4</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>3.7</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
         <v>-7</v>
       </c>
-      <c r="D3">
-        <v>3.7</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
         <v>4.25</v>
       </c>
-      <c r="F3">
-        <v>2.5</v>
-      </c>
-      <c r="G3">
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1442,25 +1527,25 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>11</v>
+        <v>7.8</v>
       </c>
       <c r="C4">
-        <v>2.9</v>
+        <v>-7</v>
       </c>
       <c r="D4">
         <v>-8.3000000000000007</v>
       </c>
       <c r="E4">
-        <v>2.9</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
         <v>2</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1468,16 +1553,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>2.9</v>
+        <v>3.7</v>
       </c>
       <c r="C5">
         <v>-7</v>
       </c>
       <c r="D5">
-        <v>0.1</v>
+        <v>3.7</v>
       </c>
       <c r="E5">
-        <v>2.9</v>
+        <v>4.25</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1486,7 +1571,7 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1494,16 +1579,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-11</v>
+        <v>11</v>
       </c>
       <c r="C6">
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="D6">
-        <v>7.2</v>
+        <v>-8.3000000000000007</v>
       </c>
       <c r="E6">
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1512,21 +1597,33 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7">
+        <v>2.9</v>
+      </c>
+      <c r="C7">
+        <v>-7</v>
+      </c>
+      <c r="D7">
+        <v>0.1</v>
+      </c>
+      <c r="E7">
+        <v>2.9</v>
+      </c>
       <c r="F7">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1534,16 +1631,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="C8">
-        <v>-2.4</v>
+        <v>3.1</v>
       </c>
       <c r="D8">
-        <v>-8.1</v>
+        <v>7.2</v>
       </c>
       <c r="E8">
-        <v>-2.4</v>
+        <v>3.1</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1552,33 +1649,21 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>1.8</v>
-      </c>
-      <c r="C9">
-        <v>7</v>
-      </c>
-      <c r="D9">
-        <v>1.8</v>
-      </c>
-      <c r="E9">
-        <v>-4</v>
-      </c>
       <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
         <v>2</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1586,16 +1671,16 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>-11</v>
+        <v>11</v>
       </c>
       <c r="C10">
-        <v>3.1</v>
+        <v>-2.4</v>
       </c>
       <c r="D10">
-        <v>6.2</v>
+        <v>-8.1</v>
       </c>
       <c r="E10">
-        <v>3.1</v>
+        <v>-2.4</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1604,7 +1689,7 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1612,25 +1697,25 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>6.2</v>
+        <v>1.8</v>
       </c>
       <c r="C11">
         <v>7</v>
       </c>
       <c r="D11">
-        <v>6.2</v>
+        <v>1.8</v>
       </c>
       <c r="E11">
-        <v>-3.45</v>
+        <v>-4</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1641,13 +1726,13 @@
         <v>-11</v>
       </c>
       <c r="C12">
-        <v>0.4</v>
+        <v>3.1</v>
       </c>
       <c r="D12">
-        <v>0.75</v>
+        <v>6.2</v>
       </c>
       <c r="E12">
-        <v>0.4</v>
+        <v>3.1</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1664,25 +1749,25 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>-4</v>
+        <v>6.2</v>
       </c>
       <c r="C13">
         <v>7</v>
       </c>
       <c r="D13">
-        <v>3.4</v>
+        <v>6.2</v>
       </c>
       <c r="E13">
-        <v>-2.2999999999999998</v>
+        <v>-3.45</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1690,16 +1775,16 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="C14">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="D14">
-        <v>-8</v>
+        <v>0.75</v>
       </c>
       <c r="E14">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1708,21 +1793,33 @@
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15">
+        <v>-4</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>3.4</v>
+      </c>
+      <c r="E15">
+        <v>-2.2999999999999998</v>
+      </c>
       <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
         <v>2</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1733,13 +1830,13 @@
         <v>11</v>
       </c>
       <c r="C16">
-        <v>1.6</v>
+        <v>0.25</v>
       </c>
       <c r="D16">
-        <v>-8.3000000000000007</v>
+        <v>-8</v>
       </c>
       <c r="E16">
-        <v>1.6</v>
+        <v>0.25</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1755,32 +1852,72 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>1.6</v>
+      </c>
+      <c r="D18">
+        <v>-8.3000000000000007</v>
+      </c>
+      <c r="E18">
+        <v>1.6</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
         <v>-11</v>
       </c>
-      <c r="C17">
+      <c r="C19">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D17">
+      <c r="D19">
         <v>2.85</v>
       </c>
-      <c r="E17">
+      <c r="E19">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F17">
-        <v>2</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H23">
       <formula1>"CircleKey,CrossKey,TriangleKey,UpArrow,DownArrow,LeftArrow"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added mari lyrics data and notes data
</commit_message>
<xml_diff>
--- a/RapZapSnap/Assets/Chew/script/Excel Related/NotesData.xlsx
+++ b/RapZapSnap/Assets/Chew/script/Excel Related/NotesData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\student\Desktop\rap.zap.snap\RapZapSnap\Assets\Chew\script\Excel Related\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20088" yWindow="0" windowWidth="8712" windowHeight="12780" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="20085" yWindow="0" windowWidth="8715" windowHeight="12780" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="tokiwa1" sheetId="1" r:id="rId1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="11">
   <si>
     <t>delaytime</t>
     <phoneticPr fontId="1"/>
@@ -66,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -148,7 +153,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -156,12 +161,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -203,7 +211,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -238,7 +246,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -453,9 +461,9 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -472,7 +480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -489,7 +497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -506,7 +514,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -523,7 +531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -540,7 +548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -557,7 +565,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -574,7 +582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -591,7 +599,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -608,7 +616,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -625,7 +633,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -642,7 +650,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11</v>
       </c>
@@ -659,7 +667,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>12</v>
       </c>
@@ -676,7 +684,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13</v>
       </c>
@@ -693,7 +701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>14</v>
       </c>
@@ -710,7 +718,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>15</v>
       </c>
@@ -727,7 +735,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>16</v>
       </c>
@@ -744,7 +752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>17</v>
       </c>
@@ -761,7 +769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>18</v>
       </c>
@@ -798,9 +806,9 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -817,7 +825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -834,7 +842,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -851,7 +859,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -868,7 +876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -885,7 +893,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -902,7 +910,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -919,7 +927,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -936,7 +944,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -953,7 +961,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -970,7 +978,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -987,7 +995,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1004,7 +1012,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1021,7 +1029,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1038,7 +1046,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1055,7 +1063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1072,7 +1080,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1089,7 +1097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1106,7 +1114,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1143,12 +1151,12 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1165,7 +1173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1182,7 +1190,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1199,7 +1207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1216,7 +1224,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1233,7 +1241,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1250,7 +1258,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1267,7 +1275,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1284,7 +1292,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1301,7 +1309,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1318,7 +1326,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1335,7 +1343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1352,7 +1360,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1369,7 +1377,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1386,7 +1394,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1403,7 +1411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1420,7 +1428,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1437,7 +1445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1454,7 +1462,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1491,9 +1499,9 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1510,7 +1518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1527,7 +1535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1544,7 +1552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1561,7 +1569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1578,7 +1586,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1595,7 +1603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1612,7 +1620,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1629,7 +1637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1646,7 +1654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1663,7 +1671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1680,7 +1688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1697,7 +1705,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1714,7 +1722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1731,7 +1739,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1748,7 +1756,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1765,7 +1773,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1782,7 +1790,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1799,7 +1807,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1835,9 +1843,9 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1854,7 +1862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1871,7 +1879,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1888,7 +1896,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1905,7 +1913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1922,7 +1930,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1939,7 +1947,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1956,7 +1964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1973,7 +1981,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1990,7 +1998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2007,7 +2015,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2024,7 +2032,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2041,7 +2049,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2058,7 +2066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2075,7 +2083,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2092,7 +2100,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2109,7 +2117,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2126,7 +2134,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2143,7 +2151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2175,13 +2183,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2198,7 +2206,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2215,7 +2223,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2232,7 +2240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2249,7 +2257,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2266,7 +2274,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2283,7 +2291,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2300,7 +2308,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2317,7 +2325,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2334,7 +2342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2351,7 +2359,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2368,7 +2376,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2385,7 +2393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2402,7 +2410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2419,7 +2427,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2436,7 +2444,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2453,7 +2461,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2470,7 +2478,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2487,7 +2495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2517,15 +2525,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E17"/>
+      <selection activeCell="C2" sqref="C2:C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2542,7 +2550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2559,7 +2567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2567,7 +2575,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -2576,7 +2584,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2584,7 +2592,7 @@
         <v>-7</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2593,7 +2601,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2601,7 +2609,7 @@
         <v>5.4</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2610,7 +2618,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2618,16 +2626,16 @@
         <v>-7</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2635,16 +2643,16 @@
         <v>5.7</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2652,16 +2660,16 @@
         <v>-7</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2669,16 +2677,16 @@
         <v>4.5</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2686,7 +2694,7 @@
         <v>-7</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2695,7 +2703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2703,7 +2711,7 @@
         <v>5.4</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2712,7 +2720,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2720,7 +2728,7 @@
         <v>-7</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2729,7 +2737,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2737,7 +2745,7 @@
         <v>5.6</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2746,7 +2754,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2754,7 +2762,7 @@
         <v>-7</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -2763,7 +2771,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2771,7 +2779,7 @@
         <v>6</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -2780,7 +2788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2788,7 +2796,7 @@
         <v>-7</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2797,7 +2805,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2805,19 +2813,41 @@
         <v>5.65</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>1.7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>0.3</v>
+      </c>
+      <c r="E19" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E19">
       <formula1>"CircleKey,CrossKey,TriangleKey,UpArrow,DownArrow,LeftArrow"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2827,15 +2857,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2852,7 +2882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2869,7 +2899,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2877,7 +2907,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -2886,7 +2916,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2894,7 +2924,7 @@
         <v>-7</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2903,7 +2933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2911,7 +2941,7 @@
         <v>5.4</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2920,7 +2950,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2928,16 +2958,16 @@
         <v>-7</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2945,16 +2975,16 @@
         <v>5.7</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2962,16 +2992,16 @@
         <v>-7</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2979,16 +3009,16 @@
         <v>4.5</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2996,7 +3026,7 @@
         <v>-7</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -3005,7 +3035,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3013,7 +3043,7 @@
         <v>5.4</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -3022,7 +3052,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3030,7 +3060,7 @@
         <v>-7</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -3039,7 +3069,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3047,7 +3077,7 @@
         <v>5.6</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -3056,7 +3086,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3064,7 +3094,7 @@
         <v>-7</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -3073,7 +3103,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3090,7 +3120,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3098,7 +3128,7 @@
         <v>-7</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -3107,7 +3137,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3121,31 +3151,54 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>0.5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>0.4</v>
+      </c>
+      <c r="E19" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E19">
       <formula1>"CircleKey,CrossKey,TriangleKey,UpArrow,DownArrow,LeftArrow"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3162,7 +3215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3179,7 +3232,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3187,7 +3240,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -3196,7 +3249,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3204,7 +3257,7 @@
         <v>-7</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -3213,7 +3266,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3221,7 +3274,7 @@
         <v>5.4</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -3230,7 +3283,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3238,16 +3291,16 @@
         <v>-7</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3255,16 +3308,16 @@
         <v>5.7</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3272,16 +3325,16 @@
         <v>-7</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3289,16 +3342,16 @@
         <v>4.5</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3306,7 +3359,7 @@
         <v>-7</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -3315,7 +3368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3323,7 +3376,7 @@
         <v>5.4</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -3332,7 +3385,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3340,7 +3393,7 @@
         <v>-7</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -3349,7 +3402,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3357,7 +3410,7 @@
         <v>5.6</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -3366,7 +3419,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3374,7 +3427,7 @@
         <v>-7</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -3383,7 +3436,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3391,7 +3444,7 @@
         <v>6</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -3400,7 +3453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3408,7 +3461,7 @@
         <v>-7</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -3417,7 +3470,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3425,19 +3478,41 @@
         <v>5.65</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>1.4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>0.3</v>
+      </c>
+      <c r="E19" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E19">
       <formula1>"CircleKey,CrossKey,TriangleKey,UpArrow,DownArrow,LeftArrow"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added mari notes speed, remove old lyrics files
</commit_message>
<xml_diff>
--- a/RapZapSnap/Assets/Chew/script/Excel Related/NotesData.xlsx
+++ b/RapZapSnap/Assets/Chew/script/Excel Related/NotesData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20085" yWindow="0" windowWidth="8715" windowHeight="12780" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="20085" yWindow="0" windowWidth="8715" windowHeight="12780" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="tokiwa1" sheetId="1" r:id="rId1"/>
@@ -2528,7 +2528,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -2561,7 +2561,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -2578,7 +2578,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -2595,7 +2595,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
@@ -2612,7 +2612,7 @@
         <v>1.5</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -2629,7 +2629,7 @@
         <v>0.8</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -2646,7 +2646,7 @@
         <v>1.2</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -2663,7 +2663,7 @@
         <v>1.2</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -2680,7 +2680,7 @@
         <v>0.8</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -2697,7 +2697,7 @@
         <v>1.3</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -2714,7 +2714,7 @@
         <v>0.5</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -2731,7 +2731,7 @@
         <v>1.6</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
@@ -2748,7 +2748,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
@@ -2765,7 +2765,7 @@
         <v>1.4</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E14" t="s">
         <v>6</v>
@@ -2782,7 +2782,7 @@
         <v>0.5</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E15" t="s">
         <v>2</v>
@@ -2799,7 +2799,7 @@
         <v>1.5</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
@@ -2816,7 +2816,7 @@
         <v>0.8</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>1.7</v>
       </c>
       <c r="E17" t="s">
         <v>2</v>
@@ -2829,6 +2829,9 @@
       <c r="C18">
         <v>1.7</v>
       </c>
+      <c r="D18">
+        <v>0.3</v>
+      </c>
       <c r="E18" t="s">
         <v>9</v>
       </c>
@@ -2839,6 +2842,9 @@
       </c>
       <c r="C19">
         <v>0.3</v>
+      </c>
+      <c r="D19">
+        <v>1.5</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -2852,6 +2858,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2859,8 +2866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -2893,7 +2900,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -2910,7 +2917,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -2927,7 +2934,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
@@ -2944,7 +2951,7 @@
         <v>1.5</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -2961,7 +2968,7 @@
         <v>1.6</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -2978,7 +2985,7 @@
         <v>0.5</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -2995,7 +3002,7 @@
         <v>1.3</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -3012,7 +3019,7 @@
         <v>0.9</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -3029,7 +3036,7 @@
         <v>1.6</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -3046,7 +3053,7 @@
         <v>0.3</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -3063,7 +3070,7 @@
         <v>1.3</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
@@ -3080,7 +3087,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
@@ -3114,7 +3121,7 @@
         <v>1</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E15" t="s">
         <v>2</v>
@@ -3161,6 +3168,9 @@
       <c r="C18">
         <v>0.5</v>
       </c>
+      <c r="D18">
+        <v>0.4</v>
+      </c>
       <c r="E18" t="s">
         <v>9</v>
       </c>
@@ -3171,6 +3181,9 @@
       </c>
       <c r="C19">
         <v>0.4</v>
+      </c>
+      <c r="D19">
+        <v>1.4</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -3184,7 +3197,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3192,7 +3205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added mari notes position
</commit_message>
<xml_diff>
--- a/RapZapSnap/Assets/Chew/script/Excel Related/NotesData.xlsx
+++ b/RapZapSnap/Assets/Chew/script/Excel Related/NotesData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20085" yWindow="0" windowWidth="8715" windowHeight="12780" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="20085" yWindow="0" windowWidth="8715" windowHeight="12780" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="tokiwa1" sheetId="1" r:id="rId1"/>
@@ -2184,7 +2184,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -2528,7 +2528,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B2" sqref="B2:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -2554,8 +2554,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>-7</v>
+      <c r="B2">
+        <v>-6</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -2571,8 +2571,8 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>5</v>
+      <c r="B3">
+        <v>6</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>
@@ -2588,7 +2588,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>-7</v>
       </c>
       <c r="C4">
@@ -2606,7 +2606,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>5.4</v>
+        <v>3.5</v>
       </c>
       <c r="C5">
         <v>1.5</v>
@@ -2640,7 +2640,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>5.7</v>
+        <v>3.85</v>
       </c>
       <c r="C7">
         <v>1.2</v>
@@ -2674,7 +2674,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>4.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C9">
         <v>0.8</v>
@@ -2708,7 +2708,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>5.4</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="C11">
         <v>0.5</v>
@@ -2742,7 +2742,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>5.6</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="C13">
         <v>1.1000000000000001</v>
@@ -2776,7 +2776,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C15">
         <v>0.5</v>
@@ -2810,7 +2810,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>5.65</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C17">
         <v>0.8</v>
@@ -2826,6 +2826,9 @@
       <c r="A18">
         <v>17</v>
       </c>
+      <c r="B18">
+        <v>-7</v>
+      </c>
       <c r="C18">
         <v>1.7</v>
       </c>
@@ -2839,6 +2842,9 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>18</v>
+      </c>
+      <c r="B19">
+        <v>5.85</v>
       </c>
       <c r="C19">
         <v>0.3</v>
@@ -2866,8 +2872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -2893,8 +2899,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>-7</v>
+      <c r="B2">
+        <v>-6</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -2910,8 +2916,8 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>5</v>
+      <c r="B3">
+        <v>6</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>
@@ -2927,7 +2933,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>-7</v>
       </c>
       <c r="C4">
@@ -2945,7 +2951,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>5.4</v>
+        <v>5.65</v>
       </c>
       <c r="C5">
         <v>1.5</v>
@@ -2979,7 +2985,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>5.7</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C7">
         <v>0.5</v>
@@ -3013,7 +3019,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>4.5</v>
+        <v>5.55</v>
       </c>
       <c r="C9">
         <v>0.9</v>
@@ -3047,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>5.4</v>
+        <v>5.5</v>
       </c>
       <c r="C11">
         <v>0.3</v>
@@ -3081,7 +3087,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>5.6</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C13">
         <v>1.1000000000000001</v>
@@ -3115,7 +3121,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>1.4</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -3149,7 +3155,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>5.65</v>
+        <v>5.2</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -3165,6 +3171,9 @@
       <c r="A18">
         <v>17</v>
       </c>
+      <c r="B18">
+        <v>-7</v>
+      </c>
       <c r="C18">
         <v>0.5</v>
       </c>
@@ -3178,6 +3187,9 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>18</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
       </c>
       <c r="C19">
         <v>0.4</v>
@@ -3205,8 +3217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -3232,8 +3244,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>-7</v>
+      <c r="B2">
+        <v>-6</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -3249,8 +3261,8 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>5</v>
+      <c r="B3">
+        <v>6</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>
@@ -3266,7 +3278,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>-7</v>
       </c>
       <c r="C4">
@@ -3284,7 +3296,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>5.4</v>
+        <v>4.25</v>
       </c>
       <c r="C5">
         <v>1.5</v>
@@ -3318,7 +3330,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>5.7</v>
+        <v>4.95</v>
       </c>
       <c r="C7">
         <v>0.8</v>
@@ -3352,7 +3364,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="C9">
         <v>0.8</v>
@@ -3386,7 +3398,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>5.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C11">
         <v>0.8</v>
@@ -3420,7 +3432,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>5.6</v>
+        <v>5.4</v>
       </c>
       <c r="C13">
         <v>0.7</v>
@@ -3454,7 +3466,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>5.4</v>
       </c>
       <c r="C15">
         <v>0.8</v>
@@ -3488,7 +3500,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>5.65</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C17">
         <v>0.7</v>
@@ -3504,6 +3516,9 @@
       <c r="A18">
         <v>17</v>
       </c>
+      <c r="B18">
+        <v>-7</v>
+      </c>
       <c r="C18">
         <v>1.4</v>
       </c>
@@ -3514,6 +3529,9 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>18</v>
+      </c>
+      <c r="B19">
+        <v>5.7</v>
       </c>
       <c r="C19">
         <v>0.3</v>

</xml_diff>